<commit_message>
Support hint and popup columns
</commit_message>
<xml_diff>
--- a/local/scenarios/cough/processes/ExampleProcess.xlsx
+++ b/local/scenarios/cough/processes/ExampleProcess.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t xml:space="preserve">Output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Popup</t>
   </si>
   <si>
     <t xml:space="preserve">time</t>
@@ -328,10 +334,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1048576"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -364,143 +370,149 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>